<commit_message>
done excel for e1-e5
</commit_message>
<xml_diff>
--- a/reports/e1.xlsx
+++ b/reports/e1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>TinkerPro IT</t>
   </si>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">POS Terminal No: </t>
   </si>
   <si>
-    <t>Date and Time Generated: July 18, 2024 06:25:05 PM</t>
+    <t>Date and Time Generated: July 20, 2024 05:58:38 PM</t>
   </si>
   <si>
     <t>User ID: A003</t>
@@ -135,24 +135,6 @@
   </si>
   <si>
     <t>Solo Parent</t>
-  </si>
-  <si>
-    <t>2024-01-01 - 2024-12-31</t>
-  </si>
-  <si>
-    <t>00000001</t>
-  </si>
-  <si>
-    <t>00000008</t>
-  </si>
-  <si>
-    <t>1,960.48</t>
-  </si>
-  <si>
-    <t>2,422.79</t>
-  </si>
-  <si>
-    <t>2,783.84</t>
   </si>
 </sst>
 </file>
@@ -961,99 +943,37 @@
       <c r="AF15" s="1"/>
     </row>
     <row r="16" spans="1:32">
-      <c r="A16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="8">
-        <v>2783.84</v>
-      </c>
-      <c r="E16" s="8">
-        <v>2783.84</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="M16" s="8">
-        <v>2.9</v>
-      </c>
-      <c r="N16" s="8">
-        <v>0.86</v>
-      </c>
-      <c r="O16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>50.16</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>500.0</v>
-      </c>
-      <c r="R16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="S16" s="8">
-        <v>553.92</v>
-      </c>
-      <c r="T16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="U16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="V16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="W16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="X16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="Y16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="Z16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="AA16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="8">
-        <v>1</v>
-      </c>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
       <c r="AF16" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add image in purchase form:
</commit_message>
<xml_diff>
--- a/reports/e1.xlsx
+++ b/reports/e1.xlsx
@@ -113,16 +113,16 @@
     <t>Serial No: 9995</t>
   </si>
   <si>
-    <t>Machine Name: DESKTOP-VJCK8A2</t>
+    <t>Machine Name: DESKTOP-GEVQTGR</t>
   </si>
   <si>
     <t xml:space="preserve">POS Terminal No: </t>
   </si>
   <si>
-    <t>Date and Time Generated: July 22, 2024 06:29:38 PM</t>
-  </si>
-  <si>
-    <t>User ID: A0003</t>
+    <t>Date and Time Generated: July 31, 2024 11:56:52 AM</t>
+  </si>
+  <si>
+    <t>User ID: A003</t>
   </si>
   <si>
     <t>SC</t>

</xml_diff>